<commit_message>
Carga git 21/03/2024 | 12:42:56.42
</commit_message>
<xml_diff>
--- a/DocumentacionDesarrollo/Tickets_Liberación/19022024 Ticket #162289/Desarrollo/ER_CheckList_Liberacion_ Incidente 162289.xlsx
+++ b/DocumentacionDesarrollo/Tickets_Liberación/19022024 Ticket #162289/Desarrollo/ER_CheckList_Liberacion_ Incidente 162289.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GER\DocumentacionDesarrollo\Tickets_Liberación\19022024 Ticket #162289\Desarrollo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03EB7C6F-EF61-4184-98EC-1DA2F3686402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07329664-A84B-49AC-870A-9D0251BE965F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2052" yWindow="1932" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VALIDACION DE LIBERACION" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>CHECK LIST LIBERACION</t>
   </si>
@@ -80,7 +80,16 @@
     <t>TI</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>Cuentas por cobrar</t>
+  </si>
+  <si>
+    <t>Problema #162289 ITIL Problem</t>
+  </si>
+  <si>
+    <t>Pedro Sanchez Martinez</t>
+  </si>
+  <si>
+    <t>2 Hrs</t>
   </si>
   <si>
     <r>
@@ -127,27 +136,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, http://gitlab.estrellaroja.com.mx/java/facturacion-api/-/merge_requests/222</t>
+      <t>, http://gitlab.estrellaroja.com.mx/java/facturacion-api/-/merge_requests/229</t>
     </r>
   </si>
   <si>
-    <t>Cuentas por cobrar</t>
-  </si>
-  <si>
-    <t>Problema #162289 ITIL Problem</t>
-  </si>
-  <si>
-    <t>Pedro Sanchez Martinez</t>
-  </si>
-  <si>
-    <t>2 Hrs</t>
+    <t xml:space="preserve">Realizar la creacion de los objetos del DB TMS "ObjetosDB.sql" </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,14 +213,6 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -301,11 +293,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -318,7 +309,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -332,30 +322,66 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -368,54 +394,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
@@ -814,8 +794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:K8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -830,143 +810,143 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
     </row>
     <row r="4" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="34"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
     </row>
     <row r="5" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
+      <c r="B5" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
     </row>
     <row r="6" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="37"/>
+      <c r="B6" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
     </row>
     <row r="7" spans="1:14" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="36">
+      <c r="B7" s="17">
         <v>45357</v>
       </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="36"/>
-      <c r="K7" s="36"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
     </row>
     <row r="8" spans="1:14" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
-      <c r="J8" s="38"/>
-      <c r="K8" s="38"/>
+      <c r="B8" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
     </row>
     <row r="9" spans="1:14" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
-      <c r="N9" s="7"/>
+      <c r="B9" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="N9" s="6"/>
     </row>
     <row r="10" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="30"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
     </row>
     <row r="11" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="10" t="s">
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="9" t="s">
         <v>8</v>
       </c>
       <c r="G11" s="2" t="s">
@@ -975,189 +955,176 @@
       <c r="H11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="31" t="s">
+      <c r="I11" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="J11" s="31"/>
-      <c r="K11" s="31"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
     </row>
     <row r="12" spans="1:14" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="11">
+      <c r="A12" s="10">
         <v>1</v>
       </c>
-      <c r="B12" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="9"/>
+      <c r="B12" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="8"/>
       <c r="G12" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="12"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="16"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="25"/>
     </row>
     <row r="13" spans="1:14" ht="109.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6"/>
-      <c r="B13" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="16"/>
+      <c r="A13" s="10">
+        <v>2</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13" s="23"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="25"/>
     </row>
     <row r="14" spans="1:14" ht="81.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="9"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="8"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="16"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="25"/>
     </row>
     <row r="15" spans="1:14" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="9"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="8"/>
       <c r="G15" s="3"/>
       <c r="H15" s="4"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="16"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="25"/>
     </row>
     <row r="16" spans="1:14" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="9"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="8"/>
       <c r="G16" s="3"/>
       <c r="H16" s="4"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="19"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="28"/>
     </row>
     <row r="17" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="9"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="8"/>
       <c r="G17" s="3"/>
       <c r="H17" s="4"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="19"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="28"/>
     </row>
     <row r="18" spans="1:11" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="8"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="7"/>
       <c r="G18" s="3"/>
       <c r="H18" s="4"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="19"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="28"/>
     </row>
     <row r="19" spans="1:11" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="8"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="7"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="19"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="28"/>
     </row>
     <row r="20" spans="1:11" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="8"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="7"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="19"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="28"/>
     </row>
     <row r="21" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="8"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="7"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="22"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="33"/>
     </row>
     <row r="22" spans="1:11" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="9"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="8"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="22"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="33"/>
     </row>
     <row r="23" spans="1:11" ht="14.4" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="A10:K10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="B9:K9"/>
-    <mergeCell ref="A3:K4"/>
-    <mergeCell ref="B5:K5"/>
-    <mergeCell ref="B7:K7"/>
-    <mergeCell ref="B6:K6"/>
-    <mergeCell ref="B8:K8"/>
     <mergeCell ref="B12:E12"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="B14:E14"/>
     <mergeCell ref="I12:K12"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="B13:E13"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="B21:E21"/>
     <mergeCell ref="B22:E22"/>
@@ -1168,6 +1135,25 @@
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="I19:K19"/>
     <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="A10:K10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="B9:K9"/>
+    <mergeCell ref="A3:K4"/>
+    <mergeCell ref="B5:K5"/>
+    <mergeCell ref="B7:K7"/>
+    <mergeCell ref="B6:K6"/>
+    <mergeCell ref="B8:K8"/>
   </mergeCells>
   <conditionalFormatting sqref="H12:H22">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
@@ -1187,6 +1173,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="e360555d-64ae-4829-82a7-71fe16609d3e" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fa2dea8d-d592-408c-957e-fb4b72547e48">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100266978E6E812D84B9774321B1A34878A" ma:contentTypeVersion="13" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="0959759624fdd493e8a88fca8f5c738e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fa2dea8d-d592-408c-957e-fb4b72547e48" xmlns:ns3="e360555d-64ae-4829-82a7-71fe16609d3e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2b74d979d07492aa7aeb19ef804d6c17" ns2:_="" ns3:_="">
     <xsd:import namespace="fa2dea8d-d592-408c-957e-fb4b72547e48"/>
@@ -1409,27 +1415,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B37E53AB-69B2-4844-A9B8-2C7EBB86B501}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e360555d-64ae-4829-82a7-71fe16609d3e"/>
+    <ds:schemaRef ds:uri="fa2dea8d-d592-408c-957e-fb4b72547e48"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="e360555d-64ae-4829-82a7-71fe16609d3e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fa2dea8d-d592-408c-957e-fb4b72547e48">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7A40E09-B9F6-4B3E-B9F5-737A1EC5D717}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0CB7BBB5-C3AF-4DDC-990B-25C485C8DB48}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1446,23 +1451,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7A40E09-B9F6-4B3E-B9F5-737A1EC5D717}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B37E53AB-69B2-4844-A9B8-2C7EBB86B501}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e360555d-64ae-4829-82a7-71fe16609d3e"/>
-    <ds:schemaRef ds:uri="fa2dea8d-d592-408c-957e-fb4b72547e48"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>